<commit_message>
Präsentation, SCRUM und Link angepasst
</commit_message>
<xml_diff>
--- a/documentation/Task9-Sprint3/scrum_v02.xlsx
+++ b/documentation/Task9-Sprint3/scrum_v02.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_25b8\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1dfb\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="11_4E29E552DF7DEE361965C1565A9BF00D45272AFB" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{4C737AB5-3F98-449E-8ED6-5FB7E4738521}"/>
+  <xr:revisionPtr revIDLastSave="318" documentId="11_4E29E552DF7DEE361965C1565A9BF00D45272AFB" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{012896AE-1505-4EA8-A9CB-2535A0AC092F}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="753" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="753" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Sprint Backlog'!$A$1:$L$42</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="186">
   <si>
     <t>Name</t>
   </si>
@@ -295,6 +295,108 @@
     <t>Effort Actual</t>
   </si>
   <si>
+    <t>Klassen bereitstellen</t>
+  </si>
+  <si>
+    <t>Klassen gemäss dem Klassendiagramm in UML erstellen und für weitere Arbeiten zur Verfügung stellen. (Noch keine Ausarbeitung der Methoden.)</t>
+  </si>
+  <si>
+    <t>allgemein</t>
+  </si>
+  <si>
+    <t>alle, mind 2</t>
+  </si>
+  <si>
+    <t>Scrum Retrospective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Scrum Retrospective am Montag vor Abschluss durchführen und die Ergebnisse schriftlich festhalten. </t>
+  </si>
+  <si>
+    <t>Seminar: Standort auf Karte anzeigen</t>
+  </si>
+  <si>
+    <t>Einfügen von einer Google-Map Karte, und auf dieser dann die Seminare anzeigen</t>
+  </si>
+  <si>
+    <t>SeminarView, SeminarPresenter, NewSeminarView, NewSeminarPresenter</t>
+  </si>
+  <si>
+    <t>Repository</t>
+  </si>
+  <si>
+    <t>FindAll verbieten in Repository und Verwendungen eliminieren</t>
+  </si>
+  <si>
+    <t>Repositorys, allgemein Backend</t>
+  </si>
+  <si>
+    <t>Präsentation</t>
+  </si>
+  <si>
+    <t>Review: Implementiertes mit ursprünglichen Design-Thinking-Ergebnissen vergleichen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seminar-Detail-View verbessern </t>
+  </si>
+  <si>
+    <t>Anzeige der Detail-View verbessern, PLZ nicht als Double darstellen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SeminarView </t>
+  </si>
+  <si>
+    <t>Setup Spring</t>
+  </si>
+  <si>
+    <t>Spring aufsetzen, damit spätestens bei der Anbindung der Datenbank diese Schnittstelle vereinfacht wird.</t>
+  </si>
+  <si>
+    <t>Datenbankanbindung</t>
+  </si>
+  <si>
+    <t>H2 anbinden, die Mock-Daten in SQL umwandeln, damit diese jeweils beim Start der Applikation geladen werden können</t>
+  </si>
+  <si>
+    <t>Repository-Klassen, Spring, H2</t>
+  </si>
+  <si>
+    <t>Layout erstellen</t>
+  </si>
+  <si>
+    <t>Unser aktuelles Layout nimmt 1/3 der Breite ein und ist dennoch zu breit (scrollbar horizontal), die Webapplikation etwas aufhübschen, damit nicht alles einfach weiss ist.</t>
+  </si>
+  <si>
+    <t>SeminarView, HomeView</t>
+  </si>
+  <si>
+    <t>Class Diagram and Persistence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die neue Modul-Aufgabe muss gelöst werden. Die Repository-Inerfaces bestehen bereits, aufgrund von Spring wird keine Implementation benötigt, ausser im Falle komplexer Querys. </t>
+  </si>
+  <si>
+    <t>Dokument auf GIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Durchführung der Präsentation und vorbereiten derer </t>
+  </si>
+  <si>
+    <t>Klassendiagramm</t>
+  </si>
+  <si>
+    <t>JPARepository nicht in unserem Package und DTO-Package verschieben, &lt;&lt;ENTITY&gt;&gt; auf allen gespeicherten Klassen hinzufügen, Neuerungen ergänzen</t>
+  </si>
+  <si>
+    <t>Screencast</t>
+  </si>
+  <si>
+    <t>Beispielvideo erstellen als Backup (abhängig von allen anderen Tasks)</t>
+  </si>
+  <si>
+    <t>Liste der Mitarbeit aus dem Scrum-Backlog erstellen (Je Komponente zusammenfassen)</t>
+  </si>
+  <si>
     <t>Seminar: Mock-Daten bereitstellen</t>
   </si>
   <si>
@@ -304,9 +406,6 @@
     <t xml:space="preserve">SeminarManager </t>
   </si>
   <si>
-    <t>alle, mind 2</t>
-  </si>
-  <si>
     <t>Seminar: GUI erstellen (noch ohne Karte)</t>
   </si>
   <si>
@@ -316,6 +415,21 @@
     <t>SeminarLayout SeminarView</t>
   </si>
   <si>
+    <t>Seminar-GUI überarbeiten</t>
+  </si>
+  <si>
+    <t>MVP umsetzen, Filter zurücksetzen, Enter-Taste implementieren, klarere Anzeige der Verfügbarkeit von Details (z.B. Info-Logo).</t>
+  </si>
+  <si>
+    <t>Seminar-Layout umgestalten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Filter sollten nach oben oder an die Seite aufklappbar, damit man den Inhalt auf den ersten Blick sieht. Buttons auf gleicher Ebene. </t>
+  </si>
+  <si>
+    <t>SeminarView</t>
+  </si>
+  <si>
     <t>Seminar: Daten validieren</t>
   </si>
   <si>
@@ -325,7 +439,7 @@
     <t>SeminarManager SeminarPresenter</t>
   </si>
   <si>
-    <t>Fertig aber nicht gemerged.</t>
+    <t xml:space="preserve">MVP umsetzen für Konstanten, Mergen. </t>
   </si>
   <si>
     <t>neues Seminar erfassen Maske erstellen</t>
@@ -337,6 +451,42 @@
     <t>SeminarLayoutCreate SeminarView</t>
   </si>
   <si>
+    <t>Seminar: Neues Seminar - Maske anpassen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elemente in der Maske nach Spring-Update korrigieren. MVP verbessern, Fehlermeldungen in der Ecke oben, Route anpassen. </t>
+  </si>
+  <si>
+    <t>Seminar: Daten abspeichern</t>
+  </si>
+  <si>
+    <t>Die Seminare sollen in der angehängten DB gespeichert werden können.</t>
+  </si>
+  <si>
+    <t>SeminarRepository, SeminarManager</t>
+  </si>
+  <si>
+    <t>Fehlermeldungen neues Seminar verbessern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keine redundanten Fehlermeldungen. </t>
+  </si>
+  <si>
+    <t>NewSeminarView, NewSeminarPresenter</t>
+  </si>
+  <si>
+    <t>Detailansicht: Link klickbar</t>
+  </si>
+  <si>
+    <t>Der Link in der Detail-Ansicht muss ein klickbarer Link sein der einen neuen Tab öffnet.</t>
+  </si>
+  <si>
+    <t>SeminarPresenter</t>
+  </si>
+  <si>
+    <t>Highlights unserer verwendeten Architektur (inkl. Coding Patterns die verwendet wurde), was könnten wir noch einsetzen</t>
+  </si>
+  <si>
     <t>Seminare: Filter Backend</t>
   </si>
   <si>
@@ -346,6 +496,12 @@
     <t>SeminarManager</t>
   </si>
   <si>
+    <t>Seminare: Filter anpassen</t>
+  </si>
+  <si>
+    <t>Keyword-Filtering anpassen. (Nicht oder sondern und) (Nur nach Titel oder Description filtern.) MVP anpassen (View muss Presenter aufrufen für Update)</t>
+  </si>
+  <si>
     <t>Seminare: Filter im GUI implementieren</t>
   </si>
   <si>
@@ -362,6 +518,12 @@
   </si>
   <si>
     <t>HomeLayout              MainView </t>
+  </si>
+  <si>
+    <t>MVP verbessern</t>
+  </si>
+  <si>
+    <t>HomeLayout MainView </t>
   </si>
   <si>
     <t>Navigation erstellen</t>
@@ -383,6 +545,15 @@
 SeminarManager</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Home-Page: Hot Topics</t>
+  </si>
+  <si>
+    <t>Auflistung der "Hot Topics" auf der Startseite implementieren</t>
+  </si>
+  <si>
     <t>Login erstellen</t>
   </si>
   <si>
@@ -392,67 +563,28 @@
     <t>LoginLayout         LoginView         UserManager UserPresenter</t>
   </si>
   <si>
+    <t>User abspeichern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die User sollen in der DB gespeichert werden. </t>
+  </si>
+  <si>
+    <t>UserManager, UserRepository</t>
+  </si>
+  <si>
     <t>Mockdaten User</t>
   </si>
   <si>
     <t>UserManager</t>
   </si>
   <si>
-    <t>Klassen bereitstellen</t>
-  </si>
-  <si>
-    <t>Klassen gemäss dem Klassendiagramm in UML erstellen und für weitere Arbeiten zur Verfügung stellen. (Noch keine Ausarbeitung der Methoden.)</t>
-  </si>
-  <si>
-    <t>allgemein</t>
-  </si>
-  <si>
-    <t>Setup Spring</t>
-  </si>
-  <si>
-    <t>Spring aufsetzen, damit spätestens bei der Anbindung der Datenbank diese Schnittstelle vereinfacht wird.</t>
-  </si>
-  <si>
-    <t>Detailansicht: Link klickbar</t>
-  </si>
-  <si>
-    <t>Der Link in der Detail-Ansicht muss ein klickbarer Link sein der einen neuen Tab öffnet.</t>
-  </si>
-  <si>
-    <t>SeminarPresenter</t>
-  </si>
-  <si>
-    <t>Seminar: Standort auf Karte anzeigen</t>
-  </si>
-  <si>
-    <t>Einfügen von einer Google-Map Karte, und auf dieser dann die Seminare anzeigen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SeminarView </t>
-  </si>
-  <si>
-    <t>Seminar: Daten abspeichern</t>
-  </si>
-  <si>
-    <t>Die Seminare sollen in der angehängten DB gespeichert werden können.</t>
-  </si>
-  <si>
-    <t>SeminarRepository, SeminarManager</t>
-  </si>
-  <si>
-    <t>Home-Page: Hot Topics</t>
-  </si>
-  <si>
-    <t>Auflistung der "Hot Topics" auf der Startseite implementieren</t>
-  </si>
-  <si>
-    <t>User abspeichern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die User sollen in der DB gespeichert werden. </t>
-  </si>
-  <si>
-    <t>UserManager, UserRepository</t>
+    <t>Passwortspeicherung verbessern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zurzeit wird das Passwort im Plain-Text gespeichert. Das soll geändert werden. </t>
+  </si>
+  <si>
+    <t>UserManager, User</t>
   </si>
   <si>
     <t>Berechtigunskonzept umsetzen</t>
@@ -462,141 +594,6 @@
   </si>
   <si>
     <t>UserManager, SeminarView, NewSeminarView</t>
-  </si>
-  <si>
-    <t>Datenbankanbindung</t>
-  </si>
-  <si>
-    <t>H2 anbinden, die Mock-Daten in SQL umwandeln, damit diese jeweils beim Start der Applikation geladen werden können</t>
-  </si>
-  <si>
-    <t>Repository-Klassen, Spring, H2</t>
-  </si>
-  <si>
-    <t>Layout erstellen</t>
-  </si>
-  <si>
-    <t>Unser aktuelles Layout nimmt 1/3 der Breite ein und ist dennoch zu breit (scrollbar horizontal), die Webapplikation etwas aufhübschen, damit nicht alles einfach weiss ist.</t>
-  </si>
-  <si>
-    <t>SeminarView, HomeView</t>
-  </si>
-  <si>
-    <t>Passwortspeicherung verbessern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zurzeit wird das Passwort im Plain-Text gespeichert. Das soll geändert werden. </t>
-  </si>
-  <si>
-    <t>UserManager, User</t>
-  </si>
-  <si>
-    <t>Seminar-GUI überarbeiten</t>
-  </si>
-  <si>
-    <t>MVP umsetzen, Filter zurücksetzen, Enter-Taste implementieren, klarere Anzeige der Verfügbarkeit von Details (z.B. Info-Logo).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MVP umsetzen für Konstanten, Mergen. </t>
-  </si>
-  <si>
-    <t>Seminar: Neues Seminar - Maske anpassen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elemente in der Maske nach Spring-Update korrigieren. MVP verbessern, Fehlermeldungen in der Ecke oben, Route anpassen. </t>
-  </si>
-  <si>
-    <t>Seminare: Filter anpassen</t>
-  </si>
-  <si>
-    <t>Keyword-Filtering anpassen. (Nicht oder sondern und) (Nur nach Titel oder Description filtern.) MVP anpassen (View muss Presenter aufrufen für Update)</t>
-  </si>
-  <si>
-    <t>MVP verbessern</t>
-  </si>
-  <si>
-    <t>HomeLayout MainView </t>
-  </si>
-  <si>
-    <t>Class Diagram and Persistence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die neue Modul-Aufgabe muss gelöst werden. Die Repository-Inerfaces bestehen bereits, aufgrund von Spring wird keine Implementation benötigt, ausser im Falle komplexer Querys. </t>
-  </si>
-  <si>
-    <t>Dokument auf GIT</t>
-  </si>
-  <si>
-    <t>Seminar-Layout umgestalten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Filter sollten nach oben oder an die Seite aufklappbar, damit man den Inhalt auf den ersten Blick sieht. Buttons auf gleicher Ebene. </t>
-  </si>
-  <si>
-    <t>Fehlermeldungen neues Seminar verbessern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keine redundanten Fehlermeldungen. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seminar-Detail-View verbessern </t>
-  </si>
-  <si>
-    <t>Anzeige der Detail-View verbessern, PLZ nicht als Double darstellen</t>
-  </si>
-  <si>
-    <t>Klassendiagramm</t>
-  </si>
-  <si>
-    <t>FindAll verbieten in Repository und Verwendungen eliminieren</t>
-  </si>
-  <si>
-    <t>JPARepository nicht in unserem Package und DTO-Package verschieben, &lt;&lt;ENTITY&gt;&gt; auf allen gespeicherten Klassen hinzufügen, Neuerungen ergänzen</t>
-  </si>
-  <si>
-    <t>Repository</t>
-  </si>
-  <si>
-    <t>Präsentation</t>
-  </si>
-  <si>
-    <t>Screencast</t>
-  </si>
-  <si>
-    <t>Beispielvideo erstellen als Backup (abhängig von allen anderen Tasks)</t>
-  </si>
-  <si>
-    <t>Review: Implementiertes mit ursprünglichen Design-Thinking-Ergebnissen vergleichen</t>
-  </si>
-  <si>
-    <t>Highlights unserer verwendeten Architektur (inkl. Coding Patterns die verwendet wurde), was könnten wir noch einsetzen</t>
-  </si>
-  <si>
-    <t>Liste der Mitarbeit aus dem Scrum-Backlog erstellen (Je Komponente zusammenfassen)</t>
-  </si>
-  <si>
-    <t>Scrum Retrospective</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Scrum Retrospective am Montag vor Abschluss durchführen und die Ergebnisse schriftlich festhalten. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Durchführung der Präsentation und vorbereiten derer </t>
-  </si>
-  <si>
-    <t>SeminarView, SeminarPresenter, NewSeminarView, NewSeminarPresenter</t>
-  </si>
-  <si>
-    <t>SeminarView</t>
-  </si>
-  <si>
-    <t>NewSeminarView, NewSeminarPresenter</t>
-  </si>
-  <si>
-    <t>Repositorys, allgemein Backend</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1877,12 +1874,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="14.45" x14ac:dyDescent="0.25"/>
@@ -1941,7 +1939,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>0.1</v>
       </c>
@@ -1949,13 +1947,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>2</v>
@@ -1978,21 +1976,21 @@
       </c>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>0.11</v>
+    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>0.15</v>
       </c>
       <c r="B3" s="8">
         <v>3</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>173</v>
+        <v>90</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>181</v>
+        <v>91</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>173</v>
+        <v>88</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>12</v>
@@ -2007,30 +2005,32 @@
         <v>1</v>
       </c>
       <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="K3" s="8">
+        <v>1</v>
+      </c>
       <c r="L3" s="8" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <v>0.12</v>
+        <v>1.3</v>
       </c>
       <c r="B4" s="8">
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>172</v>
+        <v>92</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>170</v>
+        <v>93</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>185</v>
+        <v>94</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>89</v>
@@ -2039,35 +2039,35 @@
         <v>23</v>
       </c>
       <c r="I4" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="K4" s="8">
+        <v>3</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>169</v>
+        <v>95</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>169</v>
+        <v>97</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>89</v>
@@ -2079,30 +2079,32 @@
         <v>2</v>
       </c>
       <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8" t="s">
-        <v>24</v>
+      <c r="K5" s="8">
+        <v>2</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:13" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <v>0.14000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="B6" s="8">
         <v>3</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>174</v>
+        <v>98</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>175</v>
+        <v>99</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>89</v>
@@ -2111,33 +2113,35 @@
         <v>23</v>
       </c>
       <c r="I6" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8" t="s">
-        <v>24</v>
+      <c r="K6" s="8">
+        <v>2</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <v>0.15</v>
+        <v>3.3</v>
       </c>
       <c r="B7" s="8">
         <v>3</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>180</v>
+        <v>100</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>101</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>89</v>
@@ -2146,16 +2150,18 @@
         <v>23</v>
       </c>
       <c r="I7" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8" t="s">
-        <v>24</v>
+      <c r="K7" s="8">
+        <v>2</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>0.2</v>
       </c>
@@ -2163,13 +2169,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>2</v>
@@ -2192,7 +2198,7 @@
       </c>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>0.3</v>
       </c>
@@ -2200,13 +2206,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>142</v>
+        <v>105</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>143</v>
+        <v>106</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>2</v>
@@ -2229,7 +2235,7 @@
       </c>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>0.4</v>
       </c>
@@ -2237,13 +2243,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>10</v>
@@ -2266,7 +2272,7 @@
       </c>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>0.5</v>
       </c>
@@ -2274,13 +2280,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>161</v>
+        <v>112</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>10</v>
@@ -2305,24 +2311,24 @@
       </c>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>0.6</v>
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>0.11</v>
       </c>
       <c r="B12" s="8">
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>176</v>
+        <v>114</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>89</v>
@@ -2331,33 +2337,35 @@
         <v>23</v>
       </c>
       <c r="I12" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8" t="s">
-        <v>24</v>
+      <c r="K12" s="8">
+        <v>1</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <v>0.7</v>
+        <v>0.13</v>
       </c>
       <c r="B13" s="8">
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>89</v>
@@ -2369,30 +2377,32 @@
         <v>2</v>
       </c>
       <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
+      <c r="K13" s="8">
+        <v>2</v>
+      </c>
       <c r="L13" s="8" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <v>0.8</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="B14" s="8">
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>173</v>
+        <v>117</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>177</v>
+        <v>118</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>89</v>
@@ -2401,33 +2411,35 @@
         <v>23</v>
       </c>
       <c r="I14" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
+      <c r="K14" s="8">
+        <v>1</v>
+      </c>
       <c r="L14" s="8" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="B15" s="8">
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>179</v>
+        <v>119</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>89</v>
@@ -2436,15 +2448,17 @@
         <v>23</v>
       </c>
       <c r="I15" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="K15" s="8">
+        <v>1</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>1.1000000000000001</v>
       </c>
@@ -2452,13 +2466,13 @@
         <v>1</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>6</v>
@@ -2480,7 +2494,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>1.2</v>
       </c>
@@ -2488,13 +2502,13 @@
         <v>1</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>10</v>
@@ -2516,7 +2530,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>1.2</v>
       </c>
@@ -2524,13 +2538,13 @@
         <v>2</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>10</v>
@@ -2552,24 +2566,24 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <v>1.2</v>
+        <v>0.9</v>
       </c>
       <c r="B19" s="8">
         <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>163</v>
+        <v>98</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>164</v>
+        <v>90</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>183</v>
+        <v>98</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>89</v>
@@ -2578,15 +2592,17 @@
         <v>23</v>
       </c>
       <c r="I19" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
+      <c r="K19" s="8">
+        <v>1</v>
+      </c>
       <c r="L19" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>1.3</v>
       </c>
@@ -2594,13 +2610,13 @@
         <v>2</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>6</v>
@@ -2624,9 +2640,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="B21" s="8">
         <v>3</v>
@@ -2638,10 +2654,10 @@
         <v>129</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>182</v>
+        <v>130</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>89</v>
@@ -2650,15 +2666,17 @@
         <v>23</v>
       </c>
       <c r="I21" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+      <c r="K21" s="8">
+        <v>2</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>2.1</v>
       </c>
@@ -2666,13 +2684,13 @@
         <v>1</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>8</v>
@@ -2696,7 +2714,7 @@
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
     </row>
-    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>2.1</v>
       </c>
@@ -2704,13 +2722,13 @@
         <v>2</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>8</v>
@@ -2734,7 +2752,7 @@
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
     </row>
-    <row r="24" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>2.2000000000000002</v>
       </c>
@@ -2742,13 +2760,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>6</v>
@@ -2772,7 +2790,7 @@
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>2.2000000000000002</v>
       </c>
@@ -2780,13 +2798,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>6</v>
@@ -2810,7 +2828,7 @@
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
     </row>
-    <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>2.2999999999999998</v>
       </c>
@@ -2818,13 +2836,13 @@
         <v>2</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>8</v>
@@ -2855,13 +2873,13 @@
         <v>3</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>184</v>
+        <v>145</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>8</v>
@@ -2876,13 +2894,15 @@
         <v>1</v>
       </c>
       <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
+      <c r="K27" s="8">
+        <v>1.5</v>
+      </c>
       <c r="L27" s="8" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="M27" s="8"/>
     </row>
-    <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>3.2</v>
       </c>
@@ -2890,13 +2910,13 @@
         <v>2</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>8</v>
@@ -2919,24 +2939,24 @@
       </c>
       <c r="M28" s="8"/>
     </row>
-    <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
-        <v>3.3</v>
+        <v>0.8</v>
       </c>
       <c r="B29" s="8">
         <v>3</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>167</v>
+        <v>98</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>89</v>
@@ -2948,14 +2968,16 @@
         <v>2</v>
       </c>
       <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
+      <c r="K29" s="8">
+        <v>2</v>
+      </c>
       <c r="L29" s="8" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
     </row>
-    <row r="30" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>4.0999999999999996</v>
       </c>
@@ -2963,13 +2985,13 @@
         <v>1</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>102</v>
+        <v>152</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>8</v>
@@ -2993,7 +3015,7 @@
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
     </row>
-    <row r="31" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>4.0999999999999996</v>
       </c>
@@ -3001,13 +3023,13 @@
         <v>2</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>102</v>
+        <v>152</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>8</v>
@@ -3031,7 +3053,7 @@
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
     </row>
-    <row r="32" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>4.2</v>
       </c>
@@ -3039,13 +3061,13 @@
         <v>1</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>103</v>
+        <v>155</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>104</v>
+        <v>156</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>105</v>
+        <v>157</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>10</v>
@@ -3069,7 +3091,7 @@
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
     </row>
-    <row r="33" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>16.100000000000001</v>
       </c>
@@ -3077,13 +3099,13 @@
         <v>1</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>106</v>
+        <v>158</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>107</v>
+        <v>159</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>4</v>
@@ -3107,7 +3129,7 @@
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
     </row>
-    <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>16.100000000000001</v>
       </c>
@@ -3115,13 +3137,13 @@
         <v>2</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>106</v>
+        <v>158</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>4</v>
@@ -3145,7 +3167,7 @@
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
     </row>
-    <row r="35" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>16.2</v>
       </c>
@@ -3153,13 +3175,13 @@
         <v>1</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>109</v>
+        <v>163</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>110</v>
+        <v>164</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>111</v>
+        <v>165</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>4</v>
@@ -3183,7 +3205,7 @@
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
     </row>
-    <row r="36" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>16.3</v>
       </c>
@@ -3191,13 +3213,13 @@
         <v>1</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>113</v>
+        <v>167</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>114</v>
+        <v>168</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>4</v>
@@ -3221,18 +3243,18 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
     </row>
-    <row r="37" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>16.399999999999999</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
@@ -3253,7 +3275,7 @@
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
     </row>
-    <row r="38" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>17.100000000000001</v>
       </c>
@@ -3261,13 +3283,13 @@
         <v>1</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>115</v>
+        <v>172</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>116</v>
+        <v>173</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>117</v>
+        <v>174</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>10</v>
@@ -3291,7 +3313,7 @@
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
     </row>
-    <row r="39" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>17.2</v>
       </c>
@@ -3299,13 +3321,13 @@
         <v>2</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>8</v>
@@ -3329,7 +3351,7 @@
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
     </row>
-    <row r="40" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>17.3</v>
       </c>
@@ -3337,13 +3359,13 @@
         <v>1</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>118</v>
+        <v>178</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>6</v>
@@ -3366,7 +3388,7 @@
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
     </row>
-    <row r="41" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>17.399999999999999</v>
       </c>
@@ -3374,13 +3396,13 @@
         <v>2</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>8</v>
@@ -3404,7 +3426,7 @@
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
     </row>
-    <row r="42" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>18.100000000000001</v>
       </c>
@@ -3412,13 +3434,13 @@
         <v>2</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>140</v>
+        <v>184</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>141</v>
+        <v>185</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>4</v>
@@ -3540,8 +3562,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L42" xr:uid="{00000000-0009-0000-0000-000003000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="3"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L42">
-      <sortCondition ref="A1:A42"/>
+      <sortCondition ref="L1:L42"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L21">

</xml_diff>